<commit_message>
update tenant name in TestData File from content_test to content to match
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/NewUI_NX_SignIn/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/NewUI_NX_SignIn/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AFarid\git\qa\src\test\resources\TestDataFiles\NewUI_NX_SignIn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4DC08E25-D524-4037-BEBA-905B9D6FE3FC}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF43136B-010C-4F0C-AFC1-1C45A31E281C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11265" windowHeight="4590" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="Lists" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -153,9 +152,6 @@
     <t>MicrosoftEdge</t>
   </si>
   <si>
-    <t>content_test</t>
-  </si>
-  <si>
     <t>C82103 - Chrome: Testing that sign in page icons are displayed</t>
   </si>
   <si>
@@ -226,6 +222,9 @@
   </si>
   <si>
     <t>The username or password you entered is incorrect.</t>
+  </si>
+  <si>
+    <t>content</t>
   </si>
 </sst>
 </file>
@@ -704,8 +703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1158,13 +1157,13 @@
         <v>31</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
@@ -1193,13 +1192,13 @@
         <v>32</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="D15" s="5" t="s">
         <v>54</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>55</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
@@ -1228,13 +1227,13 @@
         <v>33</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="D16" s="5" t="s">
         <v>54</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>55</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
@@ -1260,7 +1259,7 @@
     </row>
     <row r="17" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -1294,7 +1293,7 @@
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
       <c r="D18" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
@@ -1321,10 +1320,10 @@
     </row>
     <row r="19" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="6"/>
@@ -1353,10 +1352,10 @@
     </row>
     <row r="20" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="10" t="s">
         <v>47</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>48</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="6"/>
@@ -1385,10 +1384,10 @@
     </row>
     <row r="21" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="10" t="s">
         <v>49</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>50</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="6"/>
@@ -1417,10 +1416,10 @@
     </row>
     <row r="22" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="10" t="s">
         <v>51</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>52</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="6"/>
@@ -1449,7 +1448,7 @@
     </row>
     <row r="23" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
@@ -1479,10 +1478,10 @@
     </row>
     <row r="24" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>58</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>59</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="6"/>
@@ -1511,10 +1510,10 @@
     </row>
     <row r="25" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="6"/>
@@ -1571,10 +1570,10 @@
     </row>
     <row r="27" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="6"/>
@@ -1603,10 +1602,10 @@
     </row>
     <row r="28" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="6"/>
@@ -1663,10 +1662,10 @@
     </row>
     <row r="30" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="6"/>

</xml_diff>